<commit_message>
diary update chris zhang 1/23 - 1/29
</commit_message>
<xml_diff>
--- a/diaries/diary-chriszhang.xlsx
+++ b/diaries/diary-chriszhang.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -104,6 +104,30 @@
   </si>
   <si>
     <t xml:space="preserve">Complete homework assignment (analyze jpacman3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attend lecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learned about mental models and UML diagrams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The mental model is a useful abstraction layer between the model and the code and good for understanding limitations and possible mistakes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find 2 features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UML diagrams can be helpful but can be too complex to use easily. Searching for how a feature is implemented can result in going through a lot of different parts of the program.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A lot of stuff going on, but manageable</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;what day?&gt;</t>
@@ -403,7 +427,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -613,188 +637,188 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
+    <row r="14" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="n">
+        <v>43853</v>
+      </c>
+      <c r="B14" s="9" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="G14" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="10" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="87" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="n">
+        <v>43855</v>
+      </c>
+      <c r="B15" s="9" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="E15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>33</v>
-      </c>
       <c r="G15" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
diary update chris zhang week 1/30 (#248)
* homework 1 answers

* updated homework

* updated homework

* updated homework

* updated homework

* updated homework

* diary update 2/1

* diary update chris zhang 1/23 - 1/29

* diary update 2/1
</commit_message>
<xml_diff>
--- a/diaries/diary-chriszhang.xlsx
+++ b/diaries/diary-chriszhang.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="47">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -128,6 +128,18 @@
   </si>
   <si>
     <t xml:space="preserve">A lot of stuff going on, but manageable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learned more about UML diagrams and other models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choosing the right representation for the job is important</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write packet for 2 essential features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One function often branches out and touches a lot of different other parts.</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;what day?&gt;</t>
@@ -424,10 +436,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -683,148 +695,236 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
+    <row r="16" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="n">
+        <v>43860</v>
+      </c>
+      <c r="B16" s="9" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="G16" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="n">
+        <v>43862</v>
+      </c>
+      <c r="B17" s="9" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>41</v>
-      </c>
       <c r="G17" s="11" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E21" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="B22" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="D22" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="26" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
diary update week 2/6
</commit_message>
<xml_diff>
--- a/diaries/diary-chriszhang.xlsx
+++ b/diaries/diary-chriszhang.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="50">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -140,6 +140,15 @@
   </si>
   <si>
     <t xml:space="preserve">One function often branches out and touches a lot of different other parts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learned about and practiced mental simulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using examples can be a more effective way of simulating than simply reading through the code. You should also be careful to verify that code works the way it appears to.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tricky but neat</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;what day?&gt;</t>
@@ -438,8 +447,8 @@
   </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -741,188 +750,188 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="s">
+    <row r="18" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="n">
+        <v>43867</v>
+      </c>
+      <c r="B18" s="9" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="G18" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added diary entries up to 2/20
</commit_message>
<xml_diff>
--- a/diaries/diary-chriszhang.xlsx
+++ b/diaries/diary-chriszhang.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="70">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -149,6 +149,66 @@
   </si>
   <si>
     <t xml:space="preserve">Tricky but neat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5PM-8PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attend lecture, take midterm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explaining things is hard.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stressed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3PM-7PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finish group project assignment, discuss assignment 2 redo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Much of the information on our open-source project’s goals, stakeholders, etc. was available on their website. There was also a whole community of players and mailing lists that we were unaware of before.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Happy &amp; pleasantly surprised</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4PM-4:30PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team, Kaj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go over feedback for assignment 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It was helpful to be reminded of the importance of explaining diagrams and images, which was a blind spot for me. I also appreciated knowing more about the level of abstraction expected for this kind of documentation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thanks Kaj!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:30PM-5PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redo assignment 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almost done, just missing a few more details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is difficult to determine what level of detail to go into when describing something at a high level. We tried to stick to the essentials and omit minor details that would cloud the big-picture view of the features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learned about reading code in terms of architectural styles and social context</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Determining what would be useful in terms of illustrating the architecture of a program is pretty hard. It is also pretty easy to fall into the mistake of assuming an architectural style is being used when that’s not the case. Seeing some of the ways to find metrics for determining the state of an open source project was helpful.</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;what day?&gt;</t>
@@ -181,7 +241,7 @@
     <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -265,6 +325,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -318,7 +385,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -364,6 +431,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -447,8 +518,8 @@
   </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -773,165 +844,165 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
+    <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="n">
+        <v>43874</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="C19" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="E19" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="G19" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="10" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="n">
+        <v>43877</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="C20" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="E20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
+      <c r="G20" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="n">
+        <v>43879</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8" t="n">
+        <v>43880</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="n">
+        <v>43881</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="C23" s="10" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>47</v>
+        <v>28</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added diary entries up to 2/20 (#367)
</commit_message>
<xml_diff>
--- a/diaries/diary-chriszhang.xlsx
+++ b/diaries/diary-chriszhang.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="70">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -149,6 +149,66 @@
   </si>
   <si>
     <t xml:space="preserve">Tricky but neat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5PM-8PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attend lecture, take midterm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explaining things is hard.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stressed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3PM-7PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finish group project assignment, discuss assignment 2 redo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Much of the information on our open-source project’s goals, stakeholders, etc. was available on their website. There was also a whole community of players and mailing lists that we were unaware of before.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Happy &amp; pleasantly surprised</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4PM-4:30PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team, Kaj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go over feedback for assignment 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It was helpful to be reminded of the importance of explaining diagrams and images, which was a blind spot for me. I also appreciated knowing more about the level of abstraction expected for this kind of documentation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thanks Kaj!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:30PM-5PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redo assignment 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almost done, just missing a few more details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is difficult to determine what level of detail to go into when describing something at a high level. We tried to stick to the essentials and omit minor details that would cloud the big-picture view of the features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learned about reading code in terms of architectural styles and social context</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Determining what would be useful in terms of illustrating the architecture of a program is pretty hard. It is also pretty easy to fall into the mistake of assuming an architectural style is being used when that’s not the case. Seeing some of the ways to find metrics for determining the state of an open source project was helpful.</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;what day?&gt;</t>
@@ -181,7 +241,7 @@
     <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -265,6 +325,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -318,7 +385,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -364,6 +431,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -447,8 +518,8 @@
   </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -773,165 +844,165 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
+    <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="n">
+        <v>43874</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="C19" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="E19" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="G19" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="10" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="n">
+        <v>43877</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="C20" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="E20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
+      <c r="G20" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="n">
+        <v>43879</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8" t="n">
+        <v>43880</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="n">
+        <v>43881</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="C23" s="10" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>47</v>
+        <v>28</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
diary update up to 3/1
</commit_message>
<xml_diff>
--- a/diaries/diary-chriszhang.xlsx
+++ b/diaries/diary-chriszhang.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="79">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -211,6 +211,39 @@
     <t xml:space="preserve">Determining what would be useful in terms of illustrating the architecture of a program is pretty hard. It is also pretty easy to fall into the mistake of assuming an architectural style is being used when that’s not the case. Seeing some of the ways to find metrics for determining the state of an open source project was helpful.</t>
   </si>
   <si>
+    <t xml:space="preserve">2PM-7PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describe project architecture, social context, and interesting issues/pull requests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our project uses elements of but does not strictly implement a lot of different architectural styles and patterns, making an accurate architectural diagram difficult. On the other hand, the social context for the project is well-documented because of its forum archives and github metrics.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good, finished faster than expected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learned about design patterns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are a ton of design patterns out there, and it would be pretty useful to learn more of them. Good planning saves a lot of time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:00PM-7:30PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete part of homework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All of homework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;what insight(s) did you gain?&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;how did you feel during the activity?&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;what day?&gt;</t>
   </si>
   <si>
@@ -224,12 +257,6 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;what did you actually accomplish?&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;what insight(s) did you gain?&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;how did you feel during the activity?&gt;</t>
   </si>
 </sst>
 </file>
@@ -241,7 +268,7 @@
     <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -326,13 +353,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <i val="true"/>
-      <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -385,7 +405,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -431,10 +451,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -516,10 +532,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -949,7 +965,7 @@
       <c r="D23" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="10" t="s">
         <v>61</v>
       </c>
       <c r="F23" s="10" t="s">
@@ -959,41 +975,41 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="s">
+    <row r="24" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="n">
+        <v>43882</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="C24" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="E24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="G24" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E24" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10" t="s">
-        <v>63</v>
+    </row>
+    <row r="25" customFormat="false" ht="58.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="n">
+        <v>43888</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>67</v>
@@ -1002,11 +1018,55 @@
         <v>68</v>
       </c>
       <c r="G25" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="n">
+        <v>43891</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C26" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
     <row r="28" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1104,7 +1164,7 @@
     <row r="122" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="123" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="124" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="125" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G2"/>

</xml_diff>

<commit_message>
diary update for chris zhang up to 3/2 (#433)
* added diary entries up to 2/20

* diary update up to 3/1
</commit_message>
<xml_diff>
--- a/diaries/diary-chriszhang.xlsx
+++ b/diaries/diary-chriszhang.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="79">
   <si>
     <t xml:space="preserve">SWE 265P Diary</t>
   </si>
@@ -211,25 +211,52 @@
     <t xml:space="preserve">Determining what would be useful in terms of illustrating the architecture of a program is pretty hard. It is also pretty easy to fall into the mistake of assuming an architectural style is being used when that’s not the case. Seeing some of the ways to find metrics for determining the state of an open source project was helpful.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;what day?&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;what time?&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;as applicable, with whom?&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;what did you want to accomplish?&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;what did you actually accomplish?&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;what insight(s) did you gain?&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;how did you feel during the activity?&gt;</t>
+    <t xml:space="preserve">2PM-7PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describe project architecture, social context, and interesting issues/pull requests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our project uses elements of but does not strictly implement a lot of different architectural styles and patterns, making an accurate architectural diagram difficult. On the other hand, the social context for the project is well-documented because of its forum archives and github metrics.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good, finished faster than expected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learned about design patterns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are a ton of design patterns out there, and it would be pretty useful to learn more of them. Good planning saves a lot of time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:00PM-7:30PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete part of homework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All of homework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looking for design patterns was not too hard, but checking to make sure they were actually following the design pattern, and distinguishing similar design patterns, was a little difficult. We expected the issue to take a long time as well, but finished faster than expected, although we did end up switching issues in the middle.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1PM-3PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Look more at design patterns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read more of refactoringguru, watched some videos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tried to look more at design patterns and the kinds of problems they solve. Hoping they will come in handy in the future.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good, it’s nice to know I have these resources on hand for when I run into a design issue in the future</t>
   </si>
 </sst>
 </file>
@@ -241,7 +268,7 @@
     <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -326,13 +353,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <i val="true"/>
-      <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -385,7 +405,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -431,10 +451,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -516,10 +532,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H27" activeCellId="0" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -949,7 +965,7 @@
       <c r="D23" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="10" t="s">
         <v>61</v>
       </c>
       <c r="F23" s="10" t="s">
@@ -959,41 +975,41 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="s">
+    <row r="24" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="n">
+        <v>43882</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="C24" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="E24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="G24" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E24" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10" t="s">
-        <v>63</v>
+    </row>
+    <row r="25" customFormat="false" ht="58.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="n">
+        <v>43888</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>67</v>
@@ -1002,11 +1018,55 @@
         <v>68</v>
       </c>
       <c r="G25" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="n">
+        <v>43891</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C26" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="n">
+        <v>43892</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
     <row r="28" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1104,7 +1164,7 @@
     <row r="122" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="123" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="124" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="125" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G2"/>

</xml_diff>